<commit_message>
Modify size and text in the cell
</commit_message>
<xml_diff>
--- a/test-case-manual.xlsx
+++ b/test-case-manual.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloscavalcante/Documents/Upskilling/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D321186-914B-3C48-9FA7-8B1775CDD565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4368C29A-44B2-6741-97F3-03786BB06FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6220" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{7994B054-6027-854C-9895-1BC25B93FB2B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Case" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -381,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -444,6 +444,21 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -461,12 +476,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -482,36 +491,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF9B1F"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -555,13 +545,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -575,6 +558,38 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF9B1F"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -595,11 +610,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1490BD90-B886-A142-9008-F5AFC6421211}" name="Table1" displayName="Table1" ref="A2:B8" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1490BD90-B886-A142-9008-F5AFC6421211}" name="Table1" displayName="Table1" ref="A2:B8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A2:B8" xr:uid="{1490BD90-B886-A142-9008-F5AFC6421211}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{46CF2558-823D-4940-BB08-CB58C250E535}" name="Test Case Project" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{6601CBC9-C96A-5C46-BB5D-2DC878C53E34}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{46CF2558-823D-4940-BB08-CB58C250E535}" name="Test Case Project" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{6601CBC9-C96A-5C46-BB5D-2DC878C53E34}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609EC5E7-D611-F74D-8775-786A2041BB1D}">
   <dimension ref="A2:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="170" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -927,58 +942,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1048,7 +1063,7 @@
       <c r="H11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1083,7 +1098,7 @@
       <c r="H12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1118,7 +1133,7 @@
       <c r="H13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -1153,7 +1168,7 @@
       <c r="H14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="10" t="s">
         <v>47</v>
       </c>
       <c r="J14" s="1" t="s">

</xml_diff>